<commit_message>
add trip import api
</commit_message>
<xml_diff>
--- a/Application/Statics/Tour.xlsx
+++ b/Application/Statics/Tour.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\C-Sharp\test_sharp\console\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truon\Desktop\Capstone\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5C7CBB-BC35-4E66-BB95-1CBA56601C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A33A65-4DDD-47C0-91D9-FE9DA4A3DCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{45D2609A-403B-4D17-83B7-867B7165AD4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{45D2609A-403B-4D17-83B7-867B7165AD4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tour" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Id</t>
   </si>
@@ -47,61 +47,18 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Tour 4 đảo Nam Phú Quốc - 1 ngày</t>
-  </si>
-  <si>
-    <t>Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>Phú Quốc</t>
-  </si>
-  <si>
-    <t>Domestic</t>
-  </si>
-  <si>
-    <t>Với cát trắng nguyên sơ và nước màu ngọc lam, khung cảnh của Phú Quốc thực sự là một bữa tiệc cho các giác quan. Bạn sẽ đến với thiên đường Hòn Móng Tay để phơi nắng trên bãi biển xinh đẹp dưới bóng mát của hàng trăm cây cọ. Sau đó, bạn sẽ được khám phá thế giới dưới nước đầy màu sắc khi lặn tại Hòm Gầm Ghì. Sau bữa trưa ngon miệng được chuẩn bị bởi thuỷ thủ đoàn, bạn sẽ được cảm nhận bãi biển cát ngọc ngút ngàn và lặn ống thở trong làn nước trong vắt tại điểm đến cuối cùng, đó chính là Hòn Mây Rút.
-Chưa hết đâu nhé, vì hãy sẵn sàng cho hoạt động câu cá thú vị tại Hòn Thơm. Chắc chắc bạn sẽ bị mê hoặc bởi không khí biển và không gian cực "chill" tại Nam Phú Quốc đấy!</t>
-  </si>
-  <si>
     <t>Sequence</t>
   </si>
   <si>
-    <t xml:space="preserve">08:30-17:00 Đón khách </t>
-  </si>
-  <si>
-    <t>Tham quan đảo Gầm Ghì</t>
-  </si>
-  <si>
-    <t>Tham quan hòn Bườm hoặc hòn Móng Tay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tham quan hòn Mây Rút Trong và dùng bữa trưa </t>
-  </si>
-  <si>
-    <t>Trải nghiệm dịch vụ đi dưới biển Seawalker (chi phí tự túc)</t>
-  </si>
-  <si>
-    <t>Trả khách</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kết thúc tour. </t>
-  </si>
-  <si>
     <t>Longitude</t>
   </si>
   <si>
     <t>Latitude</t>
   </si>
   <si>
-    <t>ab873cb8-fa0f-4f8f-a61e-4565ca5c34a6</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
-    <t>1 day, 0 night</t>
-  </si>
-  <si>
     <t>Policy</t>
   </si>
   <si>
@@ -114,9 +71,6 @@
     <t>Vehicle</t>
   </si>
   <si>
-    <t>Boat</t>
-  </si>
-  <si>
     <t>a8e9b075-b682-4e12-e93b-08db55428f57</t>
   </si>
   <si>
@@ -132,9 +86,6 @@
     <t>ca2ebed2-ed61-4d12-e93f-08db55428f57</t>
   </si>
   <si>
-    <t>1879da82-4558-484c-e940-08db55428f57</t>
-  </si>
-  <si>
     <t>60d2cf8f-40d5-4413-e941-08db55428f57</t>
   </si>
   <si>
@@ -145,6 +96,112 @@
   </si>
   <si>
     <t>Thumbnail</t>
+  </si>
+  <si>
+    <t>7aa4fbb5-5ad0-4f02-8782-6d73d0bbcfcf</t>
+  </si>
+  <si>
+    <t>Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>5 day, 4 night</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>Thailand Full Package Tour (Bangkok, Pattaya)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:00-21:00 (Dinner) </t>
+  </si>
+  <si>
+    <t>Participants will be picked up by tour leader at Tan Son Nhat International Airport for flight check-in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upon arrival, check in hotel and rest. </t>
+  </si>
+  <si>
+    <t>06:00-21:00 (Breakfast - Lunch - Dinner)</t>
+  </si>
+  <si>
+    <t>Visit Lightning Art Museum &amp; Balloon Garden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visit Wat Phra Yai temple </t>
+  </si>
+  <si>
+    <t>Check in hotel in Pattaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enjoy complimentary Thai massage treatment in the evening </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are free to explore the city at night </t>
+  </si>
+  <si>
+    <t>Other activities are available for you to book at your own expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overnight in Pattaya </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breakfast at hotel. We will check out of hotel before we start our sightseeing for the day </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breakfast at hotel. You will then head to Coral Island by motorboat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enjoy lunch before transferring to Khao Chi Chan and witness the golden image of Buddha embedded onto the mountain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visit NongNooch Dinosaur Valley Pattaya </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check out World Gems Company and "Four regions floating market", a floating market model reconstructed for you to experience the typical cultural life of the local Thai regions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attend Alcazar Cabaret Show </t>
+  </si>
+  <si>
+    <t>Enjoy Coffee and Golden Cake</t>
+  </si>
+  <si>
+    <t>Breakfast is at hotel. Check out and return to Bangkok.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visit Modern Latex, then enjoy a buffet lunch on the 86th floor of Baiyoke Sky Tower </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then visit San Phra Phrom and enjoy shopping </t>
+  </si>
+  <si>
+    <t>Check out Big C, MBK, and Central World located at Pratunam Market</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overnight in Bangkok </t>
+  </si>
+  <si>
+    <t>06:30-21:00 (Breakfast)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breakfast is at hotel. Transfer to Chao Phraya and enjoy cruising along the river. Visit Wat Traimit, known as the Golden Buddha, and Wat Yannawa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer to the airport to fly back to Ho Chi Minh City. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">End of tour.     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There's a reason why Thailand is dearly adored by tourists all around the world. It's a country of contrasts. It's a country with an array of things happening all at once. It's a country of religion, of world-famous cuisine, of fascinating natural beauty, and of deeply interesting people.
+Satisfy your curiosity about Vietnam's neighboring country with this tour that is the introduction to Thailand. Visit sacred temples and shrines, entertaining cabaret show, gigantic shopping complexes, natural sights, and many many more. Don't forget to try authentic pad Thai, mango sticky rice, tom yum goong, and the one and only Thai iced tea that we all love and enjoy. </t>
+  </si>
+  <si>
+    <t>International tourists, people with dual citizenship, or foreigners who have yet to apply for Vietnamese citizenship should contact the tour operator to learn about the application process before booking the tour</t>
   </si>
 </sst>
 </file>
@@ -191,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -202,19 +259,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +596,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="100.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -551,8 +614,8 @@
     <col min="11" max="11" width="13.77734375" style="1" customWidth="1"/>
     <col min="12" max="12" width="37.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="45.21875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="47" style="5" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="47" style="4" customWidth="1"/>
     <col min="16" max="16" width="26.6640625" style="3" customWidth="1"/>
     <col min="17" max="17" width="31.44140625" style="3" customWidth="1"/>
     <col min="18" max="19" width="8.88671875" style="3"/>
@@ -573,7 +636,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -582,36 +645,39 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -622,10 +688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BFC24A-48D9-4344-8513-D0AA29A65831}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -635,210 +701,492 @@
   <sheetData>
     <row r="1" spans="1:1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6424C495-7847-491C-A610-E324C1EE4942}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="22.44140625" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="8"/>
+    <col min="5" max="5" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="10">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="10">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="10">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="10">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="10">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="10">
+        <v>3</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="10">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="10">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="10">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="10">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="10">
+        <v>3</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="10">
+        <v>4</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="10">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="10">
+        <v>4</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="10">
+        <v>4</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="10">
+        <v>4</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="10">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="10">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
         <v>26</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="10">
+        <v>5</v>
+      </c>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5">
-        <v>104.01398799005101</v>
-      </c>
-      <c r="D3" s="5">
-        <v>9.9117696645013993</v>
-      </c>
-      <c r="E3" s="7">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="B29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="10">
+        <v>5</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="5">
-        <v>104.02198789121999</v>
-      </c>
-      <c r="D4" s="5">
-        <v>9.9084659050175095</v>
-      </c>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="5">
-        <v>104.000064884241</v>
-      </c>
-      <c r="D5" s="5">
-        <v>9.9180715429389394</v>
-      </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5">
-        <v>103.95486945662</v>
-      </c>
-      <c r="D6" s="5">
-        <v>10.2311028787576</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="B30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3"/>
+      <c r="F30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>